<commit_message>
More work on the data file.
</commit_message>
<xml_diff>
--- a/stationData.xlsx
+++ b/stationData.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="stationData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="121">
   <si>
     <t>22nd Street</t>
   </si>
@@ -265,9 +265,6 @@
     <t>Sapperton</t>
   </si>
   <si>
-    <t>SPT</t>
-  </si>
-  <si>
     <t>Scott Road</t>
   </si>
   <si>
@@ -365,6 +362,21 @@
   </si>
   <si>
     <t>NNM-EXPO-WFRONT:JCW-EXPO-KGEORGE:JCW-EXPO-PWAYU</t>
+  </si>
+  <si>
+    <t>BRP-CAN-WFRONT:LDN-CAN-RICHBR</t>
+  </si>
+  <si>
+    <t>SAP</t>
+  </si>
+  <si>
+    <t>SAP-EXPO-WFRONT:LTC-EXPO-PWAYU</t>
+  </si>
+  <si>
+    <t>HLD-MILL-LLDOUG:GLM-MILL-VCCCL</t>
+  </si>
+  <si>
+    <t>MRD-CAN-WFRONT:ABD-CAN-RICHBR:TPL-CAN-YVRA</t>
   </si>
 </sst>
 </file>
@@ -1197,7 +1209,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1209,25 +1221,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1241,16 +1253,16 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1264,16 +1276,16 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1287,13 +1299,16 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+      <c r="G4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1307,13 +1322,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+      <c r="G5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1327,13 +1345,16 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+      <c r="G6" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1347,13 +1368,16 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="G7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1367,13 +1391,13 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1387,13 +1411,13 @@
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1407,13 +1431,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1427,13 +1451,13 @@
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1447,13 +1471,13 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1467,13 +1491,13 @@
         <v>3</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1487,13 +1511,13 @@
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1507,13 +1531,13 @@
         <v>3</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1527,13 +1551,13 @@
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1547,13 +1571,13 @@
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1567,13 +1591,13 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1587,13 +1611,13 @@
         <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1607,13 +1631,13 @@
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1627,13 +1651,13 @@
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1647,13 +1671,13 @@
         <v>3</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1667,13 +1691,13 @@
         <v>3</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1687,13 +1711,13 @@
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1707,13 +1731,13 @@
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1727,13 +1751,13 @@
         <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1747,13 +1771,13 @@
         <v>3</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1767,13 +1791,13 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1787,13 +1811,13 @@
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1807,13 +1831,13 @@
         <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1827,13 +1851,13 @@
         <v>2</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1847,13 +1871,13 @@
         <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1867,13 +1891,13 @@
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1887,13 +1911,13 @@
         <v>2</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1907,13 +1931,13 @@
         <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1927,13 +1951,13 @@
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1947,13 +1971,13 @@
         <v>2</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1967,13 +1991,13 @@
         <v>2</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1987,13 +2011,13 @@
         <v>1</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2007,13 +2031,13 @@
         <v>2</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2027,13 +2051,13 @@
         <v>2</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2047,13 +2071,13 @@
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2061,239 +2085,239 @@
         <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="C43" s="4">
         <v>2</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" t="s">
         <v>84</v>
-      </c>
-      <c r="B44" t="s">
-        <v>85</v>
       </c>
       <c r="C44" s="4">
         <v>3</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" t="s">
         <v>86</v>
-      </c>
-      <c r="B45" t="s">
-        <v>87</v>
       </c>
       <c r="C45" s="4">
         <v>2</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" t="s">
         <v>88</v>
-      </c>
-      <c r="B46" t="s">
-        <v>89</v>
       </c>
       <c r="C46" s="4">
         <v>2</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" t="s">
         <v>90</v>
-      </c>
-      <c r="B47" t="s">
-        <v>91</v>
       </c>
       <c r="C47" s="4">
         <v>1</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" t="s">
         <v>92</v>
-      </c>
-      <c r="B48" t="s">
-        <v>93</v>
       </c>
       <c r="C48" s="4">
         <v>3</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" t="s">
         <v>94</v>
-      </c>
-      <c r="B49" t="s">
-        <v>95</v>
       </c>
       <c r="C49" s="4">
         <v>2</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" t="s">
         <v>96</v>
-      </c>
-      <c r="B50" t="s">
-        <v>97</v>
       </c>
       <c r="C50" s="4">
         <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
+        <v>97</v>
+      </c>
+      <c r="B51" t="s">
         <v>98</v>
-      </c>
-      <c r="B51" t="s">
-        <v>99</v>
       </c>
       <c r="C51" s="4">
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" t="s">
         <v>100</v>
-      </c>
-      <c r="B52" t="s">
-        <v>101</v>
       </c>
       <c r="C52" s="4">
         <v>1</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" t="s">
         <v>102</v>
-      </c>
-      <c r="B53" t="s">
-        <v>103</v>
       </c>
       <c r="C53" s="4">
         <v>1</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" t="s">
         <v>104</v>
-      </c>
-      <c r="B54" t="s">
-        <v>105</v>
       </c>
       <c r="C54" s="4">
         <v>2</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed the basic data structure of the Stations/Lines.
</commit_message>
<xml_diff>
--- a/stationData.xlsx
+++ b/stationData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="168">
   <si>
     <t>22nd Street</t>
   </si>
@@ -61,15 +61,9 @@
     <t>Burquitlam</t>
   </si>
   <si>
-    <t>BQM</t>
-  </si>
-  <si>
     <t>Burrard</t>
   </si>
   <si>
-    <t>BRR</t>
-  </si>
-  <si>
     <t>Columbia</t>
   </si>
   <si>
@@ -103,9 +97,6 @@
     <t>Gilmore</t>
   </si>
   <si>
-    <t>GLM</t>
-  </si>
-  <si>
     <t>Granville</t>
   </si>
   <si>
@@ -115,18 +106,12 @@
     <t>Holdom</t>
   </si>
   <si>
-    <t>HLD</t>
-  </si>
-  <si>
     <t>Inlet Center</t>
   </si>
   <si>
     <t>INL</t>
   </si>
   <si>
-    <t>Joyce Collingwood</t>
-  </si>
-  <si>
     <t>JCW</t>
   </si>
   <si>
@@ -193,9 +178,6 @@
     <t>Metrotown</t>
   </si>
   <si>
-    <t>MTT</t>
-  </si>
-  <si>
     <t>Moody Center</t>
   </si>
   <si>
@@ -205,9 +187,6 @@
     <t>Nanaimo</t>
   </si>
   <si>
-    <t>NNM</t>
-  </si>
-  <si>
     <t>New Westminster</t>
   </si>
   <si>
@@ -229,9 +208,6 @@
     <t>Patterson</t>
   </si>
   <si>
-    <t>PTS</t>
-  </si>
-  <si>
     <t>Production Way-University</t>
   </si>
   <si>
@@ -241,9 +217,6 @@
     <t>Renfrew</t>
   </si>
   <si>
-    <t>RFW</t>
-  </si>
-  <si>
     <t>Richmond-Brighouse</t>
   </si>
   <si>
@@ -259,9 +232,6 @@
     <t>Rupert</t>
   </si>
   <si>
-    <t>RPT</t>
-  </si>
-  <si>
     <t>Sapperton</t>
   </si>
   <si>
@@ -274,9 +244,6 @@
     <t>Sea Island Center</t>
   </si>
   <si>
-    <t>SIC</t>
-  </si>
-  <si>
     <t>Sperling-Burnaby Lake</t>
   </si>
   <si>
@@ -292,9 +259,6 @@
     <t>Surrey Central</t>
   </si>
   <si>
-    <t>SRC</t>
-  </si>
-  <si>
     <t>Templeton</t>
   </si>
   <si>
@@ -361,9 +325,6 @@
     <t>EDM-EXPO-WFRONT:NWM-EXPO-KGEORGE:NWM-EXPO-PWAYU</t>
   </si>
   <si>
-    <t>NNM-EXPO-WFRONT:JCW-EXPO-KGEORGE:JCW-EXPO-PWAYU</t>
-  </si>
-  <si>
     <t>BRP-CAN-WFRONT:LDN-CAN-RICHBR</t>
   </si>
   <si>
@@ -373,10 +334,190 @@
     <t>SAP-EXPO-WFRONT:LTC-EXPO-PWAYU</t>
   </si>
   <si>
-    <t>HLD-MILL-LLDOUG:GLM-MILL-VCCCL</t>
-  </si>
-  <si>
     <t>MRD-CAN-WFRONT:ABD-CAN-RICHBR:TPL-CAN-YVRA</t>
+  </si>
+  <si>
+    <t>OLV-CAN-WFRONT:KED-CAN-RICHBR:KED-CAN-YVRA</t>
+  </si>
+  <si>
+    <t>WTF-EXPO-WFRONT:GVL-EXPO-PWAYU:GVL-EXPO-KGEORGE</t>
+  </si>
+  <si>
+    <t>SAP-EXPO-WFRONT:SCR-EXPO-KGEORGE:NWM-EXPO-WFRONT</t>
+  </si>
+  <si>
+    <t>LCL-EXPO-LLDOUG:INL-MILL-VCCCL</t>
+  </si>
+  <si>
+    <t>BTC-MILL-VCCCL:SBL-MILL-LLDOUG</t>
+  </si>
+  <si>
+    <t>CQC-MILL-LLDOUG:MDC-MILL-VCCCL</t>
+  </si>
+  <si>
+    <t>Joyce-Collingwood</t>
+  </si>
+  <si>
+    <t>BCH-CAN-WFRONT:O41-CAN-RICHBR:O41-CAN-YVRA</t>
+  </si>
+  <si>
+    <t>LCL-MILL-VCCCL</t>
+  </si>
+  <si>
+    <t>PWU-EXPO-LLDOUG:SBL-EXPO-VCCCL</t>
+  </si>
+  <si>
+    <t>O41-CAN-WFRONT:MRD-CAN-RICHBR:MRD-CAN-YVRA</t>
+  </si>
+  <si>
+    <t>RBG-CAN-RICHBR:ABD-CAN-WFRONT</t>
+  </si>
+  <si>
+    <t>LLD-MILL-LLDOUG:CQC-MILL-VCCCL</t>
+  </si>
+  <si>
+    <t>SCT-EXPO-WFRONT:CMB-EXPO-PWAYU:CMB-EXPO-KGEORGE</t>
+  </si>
+  <si>
+    <t>L49-CAN-WFRONT:BRP-CAN-RICHBR:BRP-CAN-YVRA</t>
+  </si>
+  <si>
+    <t>MDC-MILL-LLDOUG:LTC-MILL-VCCCL</t>
+  </si>
+  <si>
+    <t>29A-EXPO-KGEORGE:29A-EXPO-PWAYU:CMB-EXPO-WFRONT</t>
+  </si>
+  <si>
+    <t>CMB-EXPO-PWAYU:CMB-EXPO-KGEORGE:22S-EXPO-WFRONT</t>
+  </si>
+  <si>
+    <t>KED-CAN-WFRONT:L49-CAN-RICHBR:L49-CAN-YVRA</t>
+  </si>
+  <si>
+    <t>YRH-CAN-WFRONT:BCH-CAN-RICHBR:BCH-CAN-YVRA</t>
+  </si>
+  <si>
+    <t>LCW-MILL-VCCCL:LTC-MILL-LLDOUG:LTC-EXPO-WFRONT</t>
+  </si>
+  <si>
+    <t>LDN-CAN-WFRONT</t>
+  </si>
+  <si>
+    <t>BRD-EXPO-PWAYU:CLB-EXPO-WFRONT</t>
+  </si>
+  <si>
+    <t>CLB-EXPO-WFRONT:GTW-EXPO-KGEORGE</t>
+  </si>
+  <si>
+    <t>YVR-CAN-YVRA:TPL-CAN-WFRONT</t>
+  </si>
+  <si>
+    <t>GVL-EXPO-WFRONT:MSW-EXPO-KGEORGE:MSW-EXPO-PWAYU</t>
+  </si>
+  <si>
+    <t>GTW-EXPO-WFRONT:KGG-EXPO-KGEORGE</t>
+  </si>
+  <si>
+    <t>WTF-CAN-WFRONT:YRH-CAN-RICHBR:YRH-CAN-YVRA</t>
+  </si>
+  <si>
+    <t>CMB-MILL-LLDOUG</t>
+  </si>
+  <si>
+    <t>VAN-CAN-WFRONT:OLV-CAN-RICHBR:OLV-CAN-YVRA</t>
+  </si>
+  <si>
+    <t>BRQ</t>
+  </si>
+  <si>
+    <t>PWU-EXPO-PWAYU:BRD-EXPO-WFRONT:PWU-MILL-VCCCL:BRQ-MILL-LLDOUG</t>
+  </si>
+  <si>
+    <t>INL-MILL-LLDOUG:BRQ-MILL-VCCCL</t>
+  </si>
+  <si>
+    <t>BUR</t>
+  </si>
+  <si>
+    <t>BUR-EXPO-WFRONT:SCT-EXPO-KGEORGE:SCT-EXPO-PWAYU</t>
+  </si>
+  <si>
+    <t>BUR-EXPO-PWAYU:BUR-EXPO-KGEORGE:VAN-CAN-RICHBR:VAN-CAN-YVRA</t>
+  </si>
+  <si>
+    <t>GIL</t>
+  </si>
+  <si>
+    <t>HOL-MILL-LLDOUG:GIL-MILL-VCCCL</t>
+  </si>
+  <si>
+    <t>HOL</t>
+  </si>
+  <si>
+    <t>HOL-MILL-VCCCL:LCW-MILL-LLDOUG</t>
+  </si>
+  <si>
+    <t>22S-EXPO-KGEORGE:22S-EXPO-PWAYU:MET-EXPO-VCCCL</t>
+  </si>
+  <si>
+    <t>MET</t>
+  </si>
+  <si>
+    <t>JCW-EXPO-WFRONT:MET-EXPO-KGEORGE:MET-EXPO-PWAYU</t>
+  </si>
+  <si>
+    <t>EDM-EXPO-KGEORGE:EDM-EXPO-PWAYU:MET-EXPO-WFRONT</t>
+  </si>
+  <si>
+    <t>PAT-EXPO-KGEORGE:PAT-EXPO-PWAYU:29A-EXPO-WFRONT</t>
+  </si>
+  <si>
+    <t>ROK-EXPO-KGEORGE:ROK-EXPO-PWAYU:PAT-EXPO-WFRONT</t>
+  </si>
+  <si>
+    <t>PAT</t>
+  </si>
+  <si>
+    <t>REN</t>
+  </si>
+  <si>
+    <t>REN-MILL-VCCCL:GIL-MILL-LLDOUG</t>
+  </si>
+  <si>
+    <t>RUP-MILL-VCCCL:BTC-MILL-LLDOUG</t>
+  </si>
+  <si>
+    <t>CMB-MILL-VCCCL:RUP-MILL-LLDOUG</t>
+  </si>
+  <si>
+    <t>RUP</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>SEA-CAN-YVRA:BRP-CAN-WFRONT</t>
+  </si>
+  <si>
+    <t>SEA-CAN-WFRONT</t>
+  </si>
+  <si>
+    <t>SCR-EXPO-WFRONT:SUR-EXPO-KGEORGE</t>
+  </si>
+  <si>
+    <t>SUR-EXPO-WFRONT</t>
+  </si>
+  <si>
+    <t>SUR</t>
+  </si>
+  <si>
+    <t>NAN-EXPO-WFRONT:JCW-EXPO-KGEORGE:JCW-EXPO-PWAYU</t>
+  </si>
+  <si>
+    <t>MSW-EXPO-WFRONT:NAN-EXPO-KGEORGE:NAN-EXPO-PWAYU:VCC-MILL-VCCCL:REN-MILL-LLDOUG</t>
+  </si>
+  <si>
+    <t>NAN</t>
   </si>
 </sst>
 </file>
@@ -1209,37 +1350,37 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="4"/>
-    <col min="7" max="7" width="164.7109375" customWidth="1"/>
+    <col min="7" max="7" width="95.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1253,16 +1394,16 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1276,16 +1417,16 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1299,16 +1440,16 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1322,16 +1463,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1345,16 +1486,16 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1368,16 +1509,16 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="G7" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1391,13 +1532,16 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
+      </c>
+      <c r="G8" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1405,919 +1549,1057 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="C9" s="4">
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
+      </c>
+      <c r="G9" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
+      </c>
+      <c r="G10" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4">
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
+      </c>
+      <c r="G11" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
+      </c>
+      <c r="G12" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="4">
         <v>3</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
+      </c>
+      <c r="G13" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="4">
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
+      </c>
+      <c r="G14" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="4">
         <v>3</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
+      </c>
+      <c r="G15" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>143</v>
       </c>
       <c r="C16" s="4">
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>145</v>
       </c>
       <c r="C18" s="4">
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18" t="s">
         <v>111</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C19" s="4">
         <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" t="s">
         <v>112</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C20" s="4">
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C22" s="4">
         <v>3</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C23" s="4">
         <v>3</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C24" s="4">
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C25" s="4">
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C26" s="4">
         <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C27" s="4">
         <v>3</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C28" s="4">
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>99</v>
+      </c>
+      <c r="G28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C29" s="4">
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C30" s="4">
         <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>148</v>
       </c>
       <c r="C31" s="4">
         <v>2</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C32" s="4">
         <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G32" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>167</v>
       </c>
       <c r="C33" s="4">
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C34" s="4">
         <v>2</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C35" s="4">
         <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C36" s="4">
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>153</v>
       </c>
       <c r="C37" s="4">
         <v>2</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G37" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C38" s="4">
         <v>2</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G38" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>154</v>
       </c>
       <c r="C39" s="4">
         <v>1</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C40" s="4">
         <v>2</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G40" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C41" s="4">
         <v>2</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>81</v>
+        <v>158</v>
       </c>
       <c r="C42" s="4">
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G42" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C43" s="4">
         <v>2</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G43" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C44" s="4">
         <v>3</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>159</v>
       </c>
       <c r="C45" s="4">
         <v>2</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C46" s="4">
         <v>2</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G46" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C47" s="4">
         <v>1</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G47" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>164</v>
       </c>
       <c r="C48" s="4">
         <v>3</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G48" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C49" s="4">
         <v>2</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G49" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C50" s="4">
         <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G50" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C51" s="4">
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G51" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C52" s="4">
         <v>1</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>99</v>
+      </c>
+      <c r="G52" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C53" s="4">
         <v>1</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+        <v>100</v>
+      </c>
+      <c r="G53" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C54" s="4">
         <v>2</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
+      </c>
+      <c r="G54" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>